<commit_message>
feat : data cpd, rs, room
</commit_message>
<xml_diff>
--- a/diagnosa_x_intervensi.xlsx
+++ b/diagnosa_x_intervensi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusup/Projects/node/react/sim-cpkp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E37F9B85-2991-EC46-A20B-CA4E6347EF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3599FF-EB02-B44A-AB72-E1729D11EC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="4" xr2:uid="{810CA097-E161-4948-8238-A0A93C309FD5}"/>
   </bookViews>
@@ -24020,7 +24020,7 @@
   <dimension ref="A1:H187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix account feature and master feature
</commit_message>
<xml_diff>
--- a/diagnosa_x_intervensi.xlsx
+++ b/diagnosa_x_intervensi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusup/Projects/node/react/sim-cpkp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3599FF-EB02-B44A-AB72-E1729D11EC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FC725D-6E30-6E48-8256-FABDBBD40021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="4" xr2:uid="{810CA097-E161-4948-8238-A0A93C309FD5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="2" xr2:uid="{810CA097-E161-4948-8238-A0A93C309FD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="copy_db" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet4!$A$1:$K$271</definedName>
     <definedName name="Fuzzy_Merged_Data" localSheetId="2">Sheet4!$A$1:$K$271</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +46,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{8ABE0597-D1A2-1343-BC5C-099BBBC87201}" name="Fuzzy_Merged_Data" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/yusup/Downloads/Fuzzy_Merged_Data.csv" decimal="," thousands="." comma="1">
+    <textPr sourceFile="/Users/yusup/Downloads/Fuzzy_Merged_Data.csv" decimal="," thousands="." comma="1">
       <textFields count="11">
         <textField type="text"/>
         <textField type="text"/>
@@ -2828,7 +2829,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -2931,7 +2932,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2947,6 +2948,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3157,74 +3164,74 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3295,6 +3302,11 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3635,8 +3647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C4D204-4B2C-7E4A-8068-D572CBB59C85}">
   <dimension ref="A1:C271"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3707,7 +3719,7 @@
       <c r="B6" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="49" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6636,8 +6648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D81ADED6-DC1A-3E47-83DF-509E0A88E491}">
   <dimension ref="A1:E214"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10305,8 +10317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F803475-5415-9145-A7F9-C9B25C1F3A4E}">
   <dimension ref="A1:K271"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
+      <selection activeCell="D174" sqref="D174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10324,35 +10336,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="47"/>
-      <c r="B1" s="47" t="s">
+      <c r="A1" s="50"/>
+      <c r="B1" s="50" t="s">
         <v>258</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="50" t="s">
         <v>259</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="50" t="s">
         <v>717</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="50" t="s">
         <v>712</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="50" t="s">
         <v>713</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="50" t="s">
         <v>421</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="50" t="s">
         <v>718</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="50" t="s">
         <v>422</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="50" t="s">
         <v>423</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="50" t="s">
         <v>424</v>
       </c>
     </row>
@@ -10497,16 +10509,16 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="47" t="s">
-        <v>428</v>
-      </c>
-      <c r="B6" s="47" t="s">
+      <c r="A6" s="51" t="s">
+        <v>428</v>
+      </c>
+      <c r="B6" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="51" t="s">
         <v>719</v>
       </c>
     </row>
@@ -10721,16 +10733,16 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="51" t="s">
         <v>439</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="51" t="s">
         <v>96</v>
       </c>
     </row>
@@ -10945,16 +10957,16 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="51" t="s">
         <v>447</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C20" s="47" t="s">
+      <c r="C20" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="D20" s="47" t="s">
+      <c r="D20" s="51" t="s">
         <v>101</v>
       </c>
     </row>
@@ -11239,16 +11251,16 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="51" t="s">
         <v>456</v>
       </c>
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C29" s="47" t="s">
+      <c r="C29" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="D29" s="47" t="s">
+      <c r="D29" s="51" t="s">
         <v>27</v>
       </c>
     </row>
@@ -11323,16 +11335,16 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="51" t="s">
         <v>459</v>
       </c>
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="51" t="s">
         <v>232</v>
       </c>
-      <c r="D32" s="47" t="s">
+      <c r="D32" s="51" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11372,16 +11384,16 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="47" t="s">
+      <c r="A34" s="51" t="s">
         <v>461</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="D34" s="47" t="s">
+      <c r="D34" s="51" t="s">
         <v>33</v>
       </c>
     </row>
@@ -11421,16 +11433,16 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="51" t="s">
         <v>463</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="D36" s="47" t="s">
+      <c r="D36" s="51" t="s">
         <v>35</v>
       </c>
     </row>
@@ -11470,16 +11482,16 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="51" t="s">
         <v>465</v>
       </c>
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C38" s="47" t="s">
+      <c r="C38" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="D38" s="47" t="s">
+      <c r="D38" s="51" t="s">
         <v>37</v>
       </c>
     </row>
@@ -11589,30 +11601,30 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="47" t="s">
+      <c r="A42" s="51" t="s">
         <v>469</v>
       </c>
-      <c r="B42" s="47" t="s">
+      <c r="B42" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C42" s="47" t="s">
+      <c r="C42" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="D42" s="47" t="s">
+      <c r="D42" s="51" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="47" t="s">
+      <c r="A43" s="51" t="s">
         <v>470</v>
       </c>
-      <c r="B43" s="47" t="s">
+      <c r="B43" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C43" s="47" t="s">
+      <c r="C43" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="D43" s="47" t="s">
+      <c r="D43" s="51" t="s">
         <v>42</v>
       </c>
     </row>
@@ -11757,16 +11769,16 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="47" t="s">
+      <c r="A48" s="51" t="s">
         <v>476</v>
       </c>
-      <c r="B48" s="47" t="s">
+      <c r="B48" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C48" s="47" t="s">
+      <c r="C48" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="D48" s="47" t="s">
+      <c r="D48" s="51" t="s">
         <v>47</v>
       </c>
     </row>
@@ -11841,16 +11853,16 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="47" t="s">
+      <c r="A51" s="51" t="s">
         <v>479</v>
       </c>
-      <c r="B51" s="47" t="s">
+      <c r="B51" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C51" s="47" t="s">
+      <c r="C51" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="D51" s="47" t="s">
+      <c r="D51" s="51" t="s">
         <v>50</v>
       </c>
     </row>
@@ -11925,16 +11937,16 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="47" t="s">
+      <c r="A54" s="51" t="s">
         <v>482</v>
       </c>
-      <c r="B54" s="47" t="s">
+      <c r="B54" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C54" s="47" t="s">
+      <c r="C54" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="D54" s="47" t="s">
+      <c r="D54" s="51" t="s">
         <v>53</v>
       </c>
     </row>
@@ -11974,44 +11986,44 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" s="47" t="s">
+      <c r="A56" s="51" t="s">
         <v>484</v>
       </c>
-      <c r="B56" s="47" t="s">
+      <c r="B56" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C56" s="47" t="s">
+      <c r="C56" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="D56" s="47" t="s">
+      <c r="D56" s="51" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" s="47" t="s">
+      <c r="A57" s="51" t="s">
         <v>485</v>
       </c>
-      <c r="B57" s="47" t="s">
+      <c r="B57" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C57" s="47" t="s">
+      <c r="C57" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="D57" s="47" t="s">
+      <c r="D57" s="51" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" s="47" t="s">
+      <c r="A58" s="51" t="s">
         <v>487</v>
       </c>
-      <c r="B58" s="47" t="s">
+      <c r="B58" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C58" s="47" t="s">
+      <c r="C58" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="D58" s="47" t="s">
+      <c r="D58" s="51" t="s">
         <v>441</v>
       </c>
     </row>
@@ -12436,30 +12448,30 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="47" t="s">
+      <c r="A71" s="51" t="s">
         <v>501</v>
       </c>
-      <c r="B71" s="47" t="s">
+      <c r="B71" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C71" s="47" t="s">
+      <c r="C71" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="D71" s="47" t="s">
+      <c r="D71" s="51" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" s="47" t="s">
+      <c r="A72" s="51" t="s">
         <v>503</v>
       </c>
-      <c r="B72" s="47" t="s">
+      <c r="B72" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C72" s="47" t="s">
+      <c r="C72" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="D72" s="47" t="s">
+      <c r="D72" s="51" t="s">
         <v>71</v>
       </c>
     </row>
@@ -12499,156 +12511,156 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" s="47" t="s">
+      <c r="A74" s="51" t="s">
         <v>506</v>
       </c>
-      <c r="B74" s="47" t="s">
+      <c r="B74" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C74" s="47" t="s">
+      <c r="C74" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="D74" s="47" t="s">
+      <c r="D74" s="51" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="47" t="s">
+      <c r="A75" s="51" t="s">
         <v>507</v>
       </c>
-      <c r="B75" s="47" t="s">
+      <c r="B75" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C75" s="47" t="s">
+      <c r="C75" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="D75" s="47" t="s">
+      <c r="D75" s="51" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76" s="47" t="s">
+      <c r="A76" s="51" t="s">
         <v>508</v>
       </c>
-      <c r="B76" s="47" t="s">
+      <c r="B76" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C76" s="47" t="s">
+      <c r="C76" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="D76" s="47" t="s">
+      <c r="D76" s="51" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A77" s="47" t="s">
+      <c r="A77" s="51" t="s">
         <v>509</v>
       </c>
-      <c r="B77" s="47" t="s">
+      <c r="B77" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C77" s="47" t="s">
+      <c r="C77" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="D77" s="47" t="s">
+      <c r="D77" s="51" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="47" t="s">
+      <c r="A78" s="51" t="s">
         <v>510</v>
       </c>
-      <c r="B78" s="47" t="s">
+      <c r="B78" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C78" s="47" t="s">
+      <c r="C78" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="D78" s="47" t="s">
+      <c r="D78" s="51" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A79" s="47" t="s">
+      <c r="A79" s="51" t="s">
         <v>511</v>
       </c>
-      <c r="B79" s="47" t="s">
+      <c r="B79" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C79" s="47" t="s">
+      <c r="C79" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="D79" s="47" t="s">
+      <c r="D79" s="51" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A80" s="47" t="s">
+      <c r="A80" s="51" t="s">
         <v>512</v>
       </c>
-      <c r="B80" s="47" t="s">
+      <c r="B80" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C80" s="47" t="s">
+      <c r="C80" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="D80" s="47" t="s">
+      <c r="D80" s="51" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A81" s="47" t="s">
+      <c r="A81" s="51" t="s">
         <v>513</v>
       </c>
-      <c r="B81" s="47" t="s">
+      <c r="B81" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C81" s="47" t="s">
+      <c r="C81" s="51" t="s">
         <v>251</v>
       </c>
-      <c r="D81" s="47" t="s">
+      <c r="D81" s="51" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="47" t="s">
+      <c r="A82" s="51" t="s">
         <v>514</v>
       </c>
-      <c r="B82" s="47" t="s">
+      <c r="B82" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C82" s="47" t="s">
+      <c r="C82" s="51" t="s">
         <v>251</v>
       </c>
-      <c r="D82" s="47" t="s">
+      <c r="D82" s="51" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A83" s="47" t="s">
+      <c r="A83" s="51" t="s">
         <v>515</v>
       </c>
-      <c r="B83" s="47" t="s">
+      <c r="B83" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C83" s="47" t="s">
+      <c r="C83" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="D83" s="47" t="s">
+      <c r="D83" s="51" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A84" s="47" t="s">
+      <c r="A84" s="51" t="s">
         <v>516</v>
       </c>
-      <c r="B84" s="47" t="s">
+      <c r="B84" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C84" s="47" t="s">
+      <c r="C84" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="D84" s="47" t="s">
+      <c r="D84" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -12688,30 +12700,30 @@
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A86" s="47" t="s">
+      <c r="A86" s="51" t="s">
         <v>518</v>
       </c>
-      <c r="B86" s="47" t="s">
+      <c r="B86" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C86" s="47" t="s">
+      <c r="C86" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="D86" s="47" t="s">
+      <c r="D86" s="51" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A87" s="47" t="s">
+      <c r="A87" s="51" t="s">
         <v>519</v>
       </c>
-      <c r="B87" s="47" t="s">
+      <c r="B87" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="C87" s="47" t="s">
+      <c r="C87" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="D87" s="47" t="s">
+      <c r="D87" s="51" t="s">
         <v>86</v>
       </c>
     </row>
@@ -12891,16 +12903,16 @@
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A93" s="47" t="s">
+      <c r="A93" s="51" t="s">
         <v>525</v>
       </c>
-      <c r="B93" s="47" t="s">
+      <c r="B93" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C93" s="47" t="s">
+      <c r="C93" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="D93" s="47" t="s">
+      <c r="D93" s="51" t="s">
         <v>592</v>
       </c>
     </row>
@@ -13010,16 +13022,16 @@
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A97" s="47" t="s">
+      <c r="A97" s="51" t="s">
         <v>529</v>
       </c>
-      <c r="B97" s="47" t="s">
+      <c r="B97" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C97" s="47" t="s">
+      <c r="C97" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="D97" s="47" t="s">
+      <c r="D97" s="51" t="s">
         <v>96</v>
       </c>
     </row>
@@ -13059,16 +13071,16 @@
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A99" s="47" t="s">
+      <c r="A99" s="51" t="s">
         <v>531</v>
       </c>
-      <c r="B99" s="47" t="s">
+      <c r="B99" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C99" s="47" t="s">
+      <c r="C99" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="D99" s="47" t="s">
+      <c r="D99" s="51" t="s">
         <v>98</v>
       </c>
     </row>
@@ -13143,16 +13155,16 @@
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A102" s="47" t="s">
+      <c r="A102" s="51" t="s">
         <v>534</v>
       </c>
-      <c r="B102" s="47" t="s">
+      <c r="B102" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C102" s="47" t="s">
+      <c r="C102" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="D102" s="47" t="s">
+      <c r="D102" s="51" t="s">
         <v>101</v>
       </c>
     </row>
@@ -13297,16 +13309,16 @@
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A107" s="47" t="s">
+      <c r="A107" s="51" t="s">
         <v>539</v>
       </c>
-      <c r="B107" s="47" t="s">
+      <c r="B107" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C107" s="47" t="s">
+      <c r="C107" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="D107" s="47" t="s">
+      <c r="D107" s="51" t="s">
         <v>106</v>
       </c>
     </row>
@@ -13381,16 +13393,16 @@
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A110" s="47" t="s">
+      <c r="A110" s="51" t="s">
         <v>542</v>
       </c>
-      <c r="B110" s="47" t="s">
+      <c r="B110" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C110" s="47" t="s">
+      <c r="C110" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="D110" s="47" t="s">
+      <c r="D110" s="51" t="s">
         <v>107</v>
       </c>
     </row>
@@ -13570,16 +13582,16 @@
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A116" s="47" t="s">
+      <c r="A116" s="51" t="s">
         <v>548</v>
       </c>
-      <c r="B116" s="47" t="s">
+      <c r="B116" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C116" s="47" t="s">
+      <c r="C116" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="D116" s="47" t="s">
+      <c r="D116" s="51" t="s">
         <v>27</v>
       </c>
     </row>
@@ -13829,16 +13841,16 @@
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A124" s="47" t="s">
+      <c r="A124" s="51" t="s">
         <v>556</v>
       </c>
-      <c r="B124" s="47" t="s">
+      <c r="B124" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C124" s="47" t="s">
+      <c r="C124" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="D124" s="47" t="s">
+      <c r="D124" s="51" t="s">
         <v>119</v>
       </c>
     </row>
@@ -13913,16 +13925,16 @@
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A127" s="47" t="s">
+      <c r="A127" s="51" t="s">
         <v>559</v>
       </c>
-      <c r="B127" s="47" t="s">
+      <c r="B127" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C127" s="47" t="s">
+      <c r="C127" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="D127" s="47" t="s">
+      <c r="D127" s="51" t="s">
         <v>122</v>
       </c>
     </row>
@@ -14067,16 +14079,16 @@
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A132" s="47" t="s">
+      <c r="A132" s="51" t="s">
         <v>564</v>
       </c>
-      <c r="B132" s="47" t="s">
+      <c r="B132" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C132" s="47" t="s">
+      <c r="C132" s="51" t="s">
         <v>232</v>
       </c>
-      <c r="D132" s="47" t="s">
+      <c r="D132" s="51" t="s">
         <v>715</v>
       </c>
     </row>
@@ -14221,16 +14233,16 @@
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A137" s="47" t="s">
+      <c r="A137" s="51" t="s">
         <v>569</v>
       </c>
-      <c r="B137" s="47" t="s">
+      <c r="B137" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C137" s="47" t="s">
+      <c r="C137" s="51" t="s">
         <v>232</v>
       </c>
-      <c r="D137" s="47" t="s">
+      <c r="D137" s="51" t="s">
         <v>626</v>
       </c>
     </row>
@@ -14270,16 +14282,16 @@
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A139" s="47" t="s">
+      <c r="A139" s="51" t="s">
         <v>571</v>
       </c>
-      <c r="B139" s="47" t="s">
+      <c r="B139" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C139" s="47" t="s">
+      <c r="C139" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="D139" s="47" t="s">
+      <c r="D139" s="51" t="s">
         <v>33</v>
       </c>
     </row>
@@ -14319,16 +14331,16 @@
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A141" s="47" t="s">
+      <c r="A141" s="51" t="s">
         <v>573</v>
       </c>
-      <c r="B141" s="47" t="s">
+      <c r="B141" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C141" s="47" t="s">
+      <c r="C141" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="D141" s="47" t="s">
+      <c r="D141" s="51" t="s">
         <v>135</v>
       </c>
     </row>
@@ -14368,16 +14380,16 @@
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A143" s="47" t="s">
+      <c r="A143" s="51" t="s">
         <v>575</v>
       </c>
-      <c r="B143" s="47" t="s">
+      <c r="B143" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C143" s="47" t="s">
+      <c r="C143" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="D143" s="47" t="s">
+      <c r="D143" s="51" t="s">
         <v>35</v>
       </c>
     </row>
@@ -14487,16 +14499,16 @@
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A147" s="47" t="s">
+      <c r="A147" s="51" t="s">
         <v>580</v>
       </c>
-      <c r="B147" s="47" t="s">
+      <c r="B147" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C147" s="47" t="s">
+      <c r="C147" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="D147" s="47" t="s">
+      <c r="D147" s="51" t="s">
         <v>37</v>
       </c>
     </row>
@@ -14606,16 +14618,16 @@
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A151" s="47" t="s">
+      <c r="A151" s="51" t="s">
         <v>584</v>
       </c>
-      <c r="B151" s="47" t="s">
+      <c r="B151" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C151" s="47" t="s">
+      <c r="C151" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="D151" s="47" t="s">
+      <c r="D151" s="51" t="s">
         <v>42</v>
       </c>
     </row>
@@ -14655,16 +14667,16 @@
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A153" s="47" t="s">
+      <c r="A153" s="51" t="s">
         <v>586</v>
       </c>
-      <c r="B153" s="47" t="s">
+      <c r="B153" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C153" s="47" t="s">
+      <c r="C153" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="D153" s="47" t="s">
+      <c r="D153" s="51" t="s">
         <v>143</v>
       </c>
     </row>
@@ -14704,16 +14716,16 @@
       </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A155" s="47" t="s">
+      <c r="A155" s="51" t="s">
         <v>588</v>
       </c>
-      <c r="B155" s="47" t="s">
+      <c r="B155" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C155" s="47" t="s">
+      <c r="C155" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="D155" s="47" t="s">
+      <c r="D155" s="51" t="s">
         <v>145</v>
       </c>
     </row>
@@ -14753,16 +14765,16 @@
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A157" s="47" t="s">
+      <c r="A157" s="51" t="s">
         <v>590</v>
       </c>
-      <c r="B157" s="47" t="s">
+      <c r="B157" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C157" s="47" t="s">
+      <c r="C157" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="D157" s="47" t="s">
+      <c r="D157" s="51" t="s">
         <v>147</v>
       </c>
     </row>
@@ -14977,72 +14989,72 @@
       </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A164" s="47" t="s">
+      <c r="A164" s="51" t="s">
         <v>598</v>
       </c>
-      <c r="B164" s="47" t="s">
+      <c r="B164" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C164" s="47" t="s">
+      <c r="C164" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="D164" s="47" t="s">
+      <c r="D164" s="51" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A165" s="47" t="s">
+      <c r="A165" s="51" t="s">
         <v>599</v>
       </c>
-      <c r="B165" s="47" t="s">
+      <c r="B165" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C165" s="47" t="s">
+      <c r="C165" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="D165" s="47" t="s">
+      <c r="D165" s="51" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A166" s="47" t="s">
+      <c r="A166" s="51" t="s">
         <v>600</v>
       </c>
-      <c r="B166" s="47" t="s">
+      <c r="B166" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C166" s="47" t="s">
+      <c r="C166" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="D166" s="47" t="s">
+      <c r="D166" s="51" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A167" s="47" t="s">
+      <c r="A167" s="51" t="s">
         <v>601</v>
       </c>
-      <c r="B167" s="47" t="s">
+      <c r="B167" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C167" s="47" t="s">
+      <c r="C167" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="D167" s="47" t="s">
+      <c r="D167" s="51" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A168" s="47" t="s">
+      <c r="A168" s="51" t="s">
         <v>602</v>
       </c>
-      <c r="B168" s="47" t="s">
+      <c r="B168" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C168" s="47" t="s">
+      <c r="C168" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="D168" s="47" t="s">
+      <c r="D168" s="51" t="s">
         <v>156</v>
       </c>
     </row>
@@ -15082,16 +15094,16 @@
       </c>
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A170" s="47" t="s">
+      <c r="A170" s="51" t="s">
         <v>604</v>
       </c>
-      <c r="B170" s="47" t="s">
+      <c r="B170" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C170" s="47" t="s">
+      <c r="C170" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="D170" s="47" t="s">
+      <c r="D170" s="51" t="s">
         <v>474</v>
       </c>
     </row>
@@ -15271,16 +15283,16 @@
       </c>
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A176" s="47" t="s">
+      <c r="A176" s="51" t="s">
         <v>610</v>
       </c>
-      <c r="B176" s="47" t="s">
+      <c r="B176" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C176" s="47" t="s">
+      <c r="C176" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="D176" s="47" t="s">
+      <c r="D176" s="51" t="s">
         <v>82</v>
       </c>
     </row>
@@ -15810,16 +15822,16 @@
       </c>
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A192" s="47" t="s">
+      <c r="A192" s="51" t="s">
         <v>627</v>
       </c>
-      <c r="B192" s="47" t="s">
+      <c r="B192" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="C192" s="47" t="s">
+      <c r="C192" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="D192" s="47" t="s">
+      <c r="D192" s="51" t="s">
         <v>181</v>
       </c>
     </row>
@@ -15999,16 +16011,16 @@
       </c>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A198" s="47" t="s">
+      <c r="A198" s="51" t="s">
         <v>633</v>
       </c>
-      <c r="B198" s="47" t="s">
+      <c r="B198" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="C198" s="47" t="s">
+      <c r="C198" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="D198" s="47" t="s">
+      <c r="D198" s="51" t="s">
         <v>186</v>
       </c>
     </row>
@@ -16048,58 +16060,58 @@
       </c>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A200" s="47" t="s">
+      <c r="A200" s="51" t="s">
         <v>635</v>
       </c>
-      <c r="B200" s="47" t="s">
+      <c r="B200" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="C200" s="47" t="s">
+      <c r="C200" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="D200" s="47" t="s">
+      <c r="D200" s="51" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A201" s="47" t="s">
+      <c r="A201" s="51" t="s">
         <v>636</v>
       </c>
-      <c r="B201" s="47" t="s">
+      <c r="B201" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="C201" s="47" t="s">
+      <c r="C201" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="D201" s="47" t="s">
+      <c r="D201" s="51" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A202" s="47" t="s">
+      <c r="A202" s="51" t="s">
         <v>637</v>
       </c>
-      <c r="B202" s="47" t="s">
+      <c r="B202" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="C202" s="47" t="s">
+      <c r="C202" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="D202" s="47" t="s">
+      <c r="D202" s="51" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A203" s="47" t="s">
+      <c r="A203" s="51" t="s">
         <v>638</v>
       </c>
-      <c r="B203" s="47" t="s">
+      <c r="B203" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="C203" s="47" t="s">
+      <c r="C203" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="D203" s="47" t="s">
+      <c r="D203" s="51" t="s">
         <v>191</v>
       </c>
     </row>
@@ -16174,16 +16186,16 @@
       </c>
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A206" s="47" t="s">
+      <c r="A206" s="51" t="s">
         <v>641</v>
       </c>
-      <c r="B206" s="47" t="s">
+      <c r="B206" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="C206" s="47" t="s">
+      <c r="C206" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="D206" s="47" t="s">
+      <c r="D206" s="51" t="s">
         <v>119</v>
       </c>
     </row>
@@ -16223,16 +16235,16 @@
       </c>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A208" s="47" t="s">
+      <c r="A208" s="51" t="s">
         <v>643</v>
       </c>
-      <c r="B208" s="47" t="s">
+      <c r="B208" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="C208" s="47" t="s">
+      <c r="C208" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="D208" s="47" t="s">
+      <c r="D208" s="51" t="s">
         <v>122</v>
       </c>
     </row>
@@ -16272,16 +16284,16 @@
       </c>
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A210" s="47" t="s">
+      <c r="A210" s="51" t="s">
         <v>645</v>
       </c>
-      <c r="B210" s="47" t="s">
+      <c r="B210" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="C210" s="47" t="s">
+      <c r="C210" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="D210" s="47" t="s">
+      <c r="D210" s="51" t="s">
         <v>33</v>
       </c>
     </row>
@@ -16391,16 +16403,16 @@
       </c>
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A214" s="47" t="s">
+      <c r="A214" s="51" t="s">
         <v>649</v>
       </c>
-      <c r="B214" s="47" t="s">
+      <c r="B214" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="C214" s="47" t="s">
+      <c r="C214" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="D214" s="47" t="s">
+      <c r="D214" s="51" t="s">
         <v>86</v>
       </c>
     </row>
@@ -16440,30 +16452,30 @@
       </c>
     </row>
     <row r="216" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A216" s="47" t="s">
+      <c r="A216" s="51" t="s">
         <v>651</v>
       </c>
-      <c r="B216" s="47" t="s">
+      <c r="B216" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="C216" s="47" t="s">
+      <c r="C216" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="D216" s="47" t="s">
+      <c r="D216" s="51" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="217" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A217" s="47" t="s">
+      <c r="A217" s="51" t="s">
         <v>652</v>
       </c>
-      <c r="B217" s="47" t="s">
+      <c r="B217" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="C217" s="47" t="s">
+      <c r="C217" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="D217" s="47" t="s">
+      <c r="D217" s="51" t="s">
         <v>202</v>
       </c>
     </row>
@@ -16958,16 +16970,16 @@
       </c>
     </row>
     <row r="232" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A232" s="47" t="s">
+      <c r="A232" s="51" t="s">
         <v>671</v>
       </c>
-      <c r="B232" s="47" t="s">
+      <c r="B232" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="C232" s="47" t="s">
+      <c r="C232" s="51" t="s">
         <v>262</v>
       </c>
-      <c r="D232" s="47" t="s">
+      <c r="D232" s="51" t="s">
         <v>211</v>
       </c>
     </row>
@@ -17007,16 +17019,16 @@
       </c>
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A234" s="47" t="s">
+      <c r="A234" s="51" t="s">
         <v>673</v>
       </c>
-      <c r="B234" s="47" t="s">
+      <c r="B234" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="C234" s="47" t="s">
+      <c r="C234" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="D234" s="47" t="s">
+      <c r="D234" s="51" t="s">
         <v>35</v>
       </c>
     </row>
@@ -17091,16 +17103,16 @@
       </c>
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A237" s="47" t="s">
+      <c r="A237" s="51" t="s">
         <v>676</v>
       </c>
-      <c r="B237" s="47" t="s">
+      <c r="B237" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="C237" s="47" t="s">
+      <c r="C237" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="D237" s="47" t="s">
+      <c r="D237" s="51" t="s">
         <v>53</v>
       </c>
     </row>
@@ -17140,16 +17152,16 @@
       </c>
     </row>
     <row r="239" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A239" s="47" t="s">
+      <c r="A239" s="51" t="s">
         <v>678</v>
       </c>
-      <c r="B239" s="47" t="s">
+      <c r="B239" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="C239" s="47" t="s">
+      <c r="C239" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="D239" s="47" t="s">
+      <c r="D239" s="51" t="s">
         <v>55</v>
       </c>
     </row>
@@ -17504,16 +17516,16 @@
       </c>
     </row>
     <row r="250" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A250" s="47" t="s">
+      <c r="A250" s="51" t="s">
         <v>689</v>
       </c>
-      <c r="B250" s="47" t="s">
+      <c r="B250" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="C250" s="47" t="s">
+      <c r="C250" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="D250" s="47" t="s">
+      <c r="D250" s="51" t="s">
         <v>225</v>
       </c>
     </row>
@@ -17588,44 +17600,44 @@
       </c>
     </row>
     <row r="253" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A253" s="47" t="s">
+      <c r="A253" s="51" t="s">
         <v>692</v>
       </c>
-      <c r="B253" s="47" t="s">
+      <c r="B253" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="C253" s="47" t="s">
+      <c r="C253" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="D253" s="47" t="s">
+      <c r="D253" s="51" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="254" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A254" s="47" t="s">
+      <c r="A254" s="51" t="s">
         <v>693</v>
       </c>
-      <c r="B254" s="47" t="s">
+      <c r="B254" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="C254" s="47" t="s">
+      <c r="C254" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="D254" s="47" t="s">
+      <c r="D254" s="51" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="255" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A255" s="47" t="s">
+      <c r="A255" s="51" t="s">
         <v>694</v>
       </c>
-      <c r="B255" s="47" t="s">
+      <c r="B255" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="C255" s="47" t="s">
+      <c r="C255" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="D255" s="47" t="s">
+      <c r="D255" s="51" t="s">
         <v>486</v>
       </c>
     </row>
@@ -17665,30 +17677,30 @@
       </c>
     </row>
     <row r="257" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A257" s="47" t="s">
+      <c r="A257" s="51" t="s">
         <v>696</v>
       </c>
-      <c r="B257" s="47" t="s">
+      <c r="B257" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="C257" s="47" t="s">
+      <c r="C257" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="D257" s="47" t="s">
+      <c r="D257" s="51" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="258" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A258" s="47" t="s">
+      <c r="A258" s="51" t="s">
         <v>697</v>
       </c>
-      <c r="B258" s="47" t="s">
+      <c r="B258" s="51" t="s">
         <v>253</v>
       </c>
-      <c r="C258" s="47" t="s">
+      <c r="C258" s="51" t="s">
         <v>232</v>
       </c>
-      <c r="D258" s="47" t="s">
+      <c r="D258" s="51" t="s">
         <v>498</v>
       </c>
     </row>
@@ -17798,16 +17810,16 @@
       </c>
     </row>
     <row r="262" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A262" s="47" t="s">
+      <c r="A262" s="51" t="s">
         <v>701</v>
       </c>
-      <c r="B262" s="47" t="s">
+      <c r="B262" s="51" t="s">
         <v>253</v>
       </c>
-      <c r="C262" s="47" t="s">
+      <c r="C262" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="D262" s="47" t="s">
+      <c r="D262" s="51" t="s">
         <v>441</v>
       </c>
     </row>
@@ -17847,30 +17859,30 @@
       </c>
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A264" s="47" t="s">
+      <c r="A264" s="51" t="s">
         <v>703</v>
       </c>
-      <c r="B264" s="47" t="s">
+      <c r="B264" s="51" t="s">
         <v>253</v>
       </c>
-      <c r="C264" s="47" t="s">
+      <c r="C264" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="D264" s="47" t="s">
+      <c r="D264" s="51" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="265" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A265" s="47" t="s">
+      <c r="A265" s="51" t="s">
         <v>705</v>
       </c>
-      <c r="B265" s="47" t="s">
+      <c r="B265" s="51" t="s">
         <v>253</v>
       </c>
-      <c r="C265" s="47" t="s">
+      <c r="C265" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="D265" s="47" t="s">
+      <c r="D265" s="51" t="s">
         <v>502</v>
       </c>
     </row>
@@ -17945,16 +17957,16 @@
       </c>
     </row>
     <row r="268" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A268" s="47" t="s">
+      <c r="A268" s="51" t="s">
         <v>708</v>
       </c>
-      <c r="B268" s="47" t="s">
+      <c r="B268" s="51" t="s">
         <v>253</v>
       </c>
-      <c r="C268" s="47" t="s">
+      <c r="C268" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="D268" s="47" t="s">
+      <c r="D268" s="51" t="s">
         <v>504</v>
       </c>
     </row>
@@ -18029,20 +18041,21 @@
       </c>
     </row>
     <row r="271" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A271" s="47" t="s">
+      <c r="A271" s="51" t="s">
         <v>711</v>
       </c>
-      <c r="B271" s="47" t="s">
+      <c r="B271" s="51" t="s">
         <v>253</v>
       </c>
-      <c r="C271" s="47" t="s">
+      <c r="C271" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="D271" s="47" t="s">
+      <c r="D271" s="51" t="s">
         <v>244</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K271" xr:uid="{1F803475-5415-9145-A7F9-C9B25C1F3A4E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -24019,7 +24032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E054AB5-2273-2340-87EF-D763046EC5F2}">
   <dimension ref="A1:H187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>